<commit_message>
Signed-off-by: Nguyễn Văn Khôi <khoi.nguyen@toancausoft.com.vn>
</commit_message>
<xml_diff>
--- a/Yeu Cau Xu ly/YeuCau.xlsx
+++ b/Yeu Cau Xu ly/YeuCau.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Yêu cầu</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Ưu tiên</t>
   </si>
   <si>
-    <t>Đang làm</t>
-  </si>
-  <si>
     <t>Trạng thái
  thực hiện</t>
   </si>
@@ -62,6 +59,15 @@
   </si>
   <si>
     <t>table medibvmmyy.d_thanhtoan trong các schema tháng năm điều reference foreign key đến table medibv0813.d_nhapll, nên không insert dữ liệu vào d_thanhtoan được</t>
+  </si>
+  <si>
+    <t>Bệnh Viện</t>
+  </si>
+  <si>
+    <t>Bình Phước</t>
+  </si>
+  <si>
+    <t>Hoàn thành</t>
   </si>
 </sst>
 </file>
@@ -475,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I96"/>
+  <dimension ref="A2:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -488,14 +494,14 @@
     <col min="3" max="3" width="31" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="3" customWidth="1"/>
     <col min="5" max="5" width="18" style="4" customWidth="1"/>
-    <col min="6" max="6" width="34" style="4" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="13" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="6" max="7" width="34" style="4" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="28.5">
+    <row r="2" spans="1:10" ht="28.5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -515,41 +521,47 @@
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
+      <c r="I2" s="8" t="s">
+        <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="87.75" customHeight="1">
+    <row r="3" spans="1:10" ht="87.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>14</v>
+      <c r="G3" s="7" t="s">
+        <v>15</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="9" t="s">
-        <v>9</v>
+      <c r="H3" s="6"/>
+      <c r="I3" s="9" t="s">
+        <v>16</v>
       </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="6"/>
       <c r="B4" s="2"/>
       <c r="C4" s="6"/>
@@ -557,10 +569,11 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="H4" s="6"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="6"/>
       <c r="B5" s="2"/>
       <c r="C5" s="6"/>
@@ -568,10 +581,11 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="H5" s="6"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="6"/>
       <c r="B6" s="2"/>
       <c r="C6" s="6"/>
@@ -579,10 +593,11 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="H6" s="6"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="6"/>
       <c r="B7" s="2"/>
       <c r="C7" s="6"/>
@@ -590,10 +605,11 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="H7" s="6"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="6"/>
       <c r="B8" s="2"/>
       <c r="C8" s="6"/>
@@ -601,10 +617,11 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="H8" s="6"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="6"/>
       <c r="B9" s="2"/>
       <c r="C9" s="6"/>
@@ -612,10 +629,11 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="H9" s="6"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="6"/>
       <c r="B10" s="2"/>
       <c r="C10" s="6"/>
@@ -623,10 +641,11 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="H10" s="6"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="6"/>
       <c r="B11" s="2"/>
       <c r="C11" s="6"/>
@@ -634,10 +653,11 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="H11" s="6"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="6"/>
       <c r="B12" s="2"/>
       <c r="C12" s="6"/>
@@ -645,10 +665,11 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="H12" s="6"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="6"/>
       <c r="B13" s="2"/>
       <c r="C13" s="6"/>
@@ -656,10 +677,11 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="H13" s="6"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="6"/>
       <c r="B14" s="2"/>
       <c r="C14" s="6"/>
@@ -667,10 +689,11 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="H14" s="6"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="6"/>
       <c r="B15" s="2"/>
       <c r="C15" s="6"/>
@@ -678,10 +701,11 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="H15" s="6"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="6"/>
       <c r="B16" s="2"/>
       <c r="C16" s="6"/>
@@ -689,10 +713,11 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="H16" s="6"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="6"/>
       <c r="B17" s="2"/>
       <c r="C17" s="6"/>
@@ -700,10 +725,11 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="H17" s="6"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="6"/>
       <c r="B18" s="2"/>
       <c r="C18" s="6"/>
@@ -711,10 +737,11 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="H18" s="6"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="6"/>
       <c r="B19" s="2"/>
       <c r="C19" s="6"/>
@@ -722,10 +749,11 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="H19" s="6"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="6"/>
       <c r="B20" s="2"/>
       <c r="C20" s="6"/>
@@ -733,10 +761,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="H20" s="6"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="6"/>
       <c r="B21" s="2"/>
       <c r="C21" s="6"/>
@@ -744,10 +773,11 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="H21" s="6"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="6"/>
       <c r="B22" s="2"/>
       <c r="C22" s="6"/>
@@ -755,10 +785,11 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="H22" s="6"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="6"/>
       <c r="B23" s="2"/>
       <c r="C23" s="6"/>
@@ -766,10 +797,11 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="H23" s="6"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="6"/>
       <c r="B24" s="2"/>
       <c r="C24" s="6"/>
@@ -777,10 +809,11 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="H24" s="6"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="6"/>
       <c r="B25" s="2"/>
       <c r="C25" s="6"/>
@@ -788,10 +821,11 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="H25" s="6"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="6"/>
       <c r="B26" s="2"/>
       <c r="C26" s="6"/>
@@ -799,10 +833,11 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="H26" s="6"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="6"/>
       <c r="B27" s="2"/>
       <c r="C27" s="6"/>
@@ -810,10 +845,11 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="H27" s="6"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="6"/>
       <c r="B28" s="2"/>
       <c r="C28" s="6"/>
@@ -821,10 +857,11 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="H28" s="6"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="6"/>
       <c r="B29" s="2"/>
       <c r="C29" s="6"/>
@@ -832,10 +869,11 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="H29" s="6"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="6"/>
       <c r="B30" s="2"/>
       <c r="C30" s="6"/>
@@ -843,10 +881,11 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="6"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="H30" s="6"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="6"/>
       <c r="B31" s="2"/>
       <c r="C31" s="6"/>
@@ -854,10 +893,11 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="6"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="H31" s="6"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="6"/>
       <c r="B32" s="2"/>
       <c r="C32" s="6"/>
@@ -865,10 +905,11 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="6"/>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="H32" s="6"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="6"/>
       <c r="B33" s="2"/>
       <c r="C33" s="6"/>
@@ -876,10 +917,11 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="6"/>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="H33" s="6"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="6"/>
       <c r="B34" s="2"/>
       <c r="C34" s="6"/>
@@ -887,10 +929,11 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="6"/>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="H34" s="6"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="6"/>
       <c r="B35" s="2"/>
       <c r="C35" s="6"/>
@@ -898,10 +941,11 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="6"/>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="H35" s="6"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="6"/>
       <c r="B36" s="2"/>
       <c r="C36" s="6"/>
@@ -909,10 +953,11 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="6"/>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="H36" s="6"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="6"/>
       <c r="B37" s="2"/>
       <c r="C37" s="6"/>
@@ -920,10 +965,11 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="6"/>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="H37" s="6"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="6"/>
       <c r="B38" s="2"/>
       <c r="C38" s="6"/>
@@ -931,10 +977,11 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="6"/>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="H38" s="6"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="6"/>
       <c r="B39" s="2"/>
       <c r="C39" s="6"/>
@@ -942,10 +989,11 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="6"/>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="H39" s="6"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="6"/>
       <c r="B40" s="2"/>
       <c r="C40" s="6"/>
@@ -953,10 +1001,11 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="6"/>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="H40" s="6"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="6"/>
       <c r="B41" s="2"/>
       <c r="C41" s="6"/>
@@ -964,10 +1013,11 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="6"/>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="H41" s="6"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="6"/>
       <c r="B42" s="2"/>
       <c r="C42" s="6"/>
@@ -975,10 +1025,11 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="6"/>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="H42" s="6"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="6"/>
       <c r="B43" s="2"/>
       <c r="C43" s="6"/>
@@ -986,10 +1037,11 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="6"/>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="H43" s="6"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="6"/>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="6"/>
       <c r="B44" s="2"/>
       <c r="C44" s="6"/>
@@ -997,10 +1049,11 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="6"/>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="H44" s="6"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="6"/>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="6"/>
       <c r="B45" s="2"/>
       <c r="C45" s="6"/>
@@ -1008,10 +1061,11 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="6"/>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="H45" s="6"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="6"/>
       <c r="B46" s="2"/>
       <c r="C46" s="6"/>
@@ -1019,10 +1073,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="6"/>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="H46" s="6"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="6"/>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="6"/>
       <c r="B47" s="2"/>
       <c r="C47" s="6"/>
@@ -1030,10 +1085,11 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="6"/>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="H47" s="6"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="6"/>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="6"/>
       <c r="B48" s="2"/>
       <c r="C48" s="6"/>
@@ -1041,10 +1097,11 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="6"/>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="H48" s="6"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="6"/>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="6"/>
       <c r="B49" s="2"/>
       <c r="C49" s="6"/>
@@ -1052,10 +1109,11 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="6"/>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="H49" s="6"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="6"/>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="6"/>
       <c r="B50" s="2"/>
       <c r="C50" s="6"/>
@@ -1063,10 +1121,11 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="6"/>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="H50" s="6"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="6"/>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="6"/>
       <c r="B51" s="2"/>
       <c r="C51" s="6"/>
@@ -1074,10 +1133,11 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="6"/>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="H51" s="6"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="6"/>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="6"/>
       <c r="B52" s="2"/>
       <c r="C52" s="6"/>
@@ -1085,10 +1145,11 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="6"/>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="H52" s="6"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="6"/>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="6"/>
       <c r="B53" s="2"/>
       <c r="C53" s="6"/>
@@ -1096,10 +1157,11 @@
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="6"/>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="H53" s="6"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="6"/>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="6"/>
       <c r="B54" s="2"/>
       <c r="C54" s="6"/>
@@ -1107,10 +1169,11 @@
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="6"/>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="H54" s="6"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="6"/>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="6"/>
       <c r="B55" s="2"/>
       <c r="C55" s="6"/>
@@ -1118,10 +1181,11 @@
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="6"/>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="H55" s="6"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="6"/>
       <c r="B56" s="2"/>
       <c r="C56" s="6"/>
@@ -1129,10 +1193,11 @@
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="6"/>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="H56" s="6"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="6"/>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="6"/>
       <c r="B57" s="2"/>
       <c r="C57" s="6"/>
@@ -1140,10 +1205,11 @@
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="6"/>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="H57" s="6"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="6"/>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="6"/>
       <c r="B58" s="2"/>
       <c r="C58" s="6"/>
@@ -1151,10 +1217,11 @@
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="6"/>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="H58" s="6"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="6"/>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="6"/>
       <c r="B59" s="2"/>
       <c r="C59" s="6"/>
@@ -1162,10 +1229,11 @@
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="6"/>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="H59" s="6"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="6"/>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="6"/>
       <c r="B60" s="2"/>
       <c r="C60" s="6"/>
@@ -1173,10 +1241,11 @@
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="6"/>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="H60" s="6"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="6"/>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="6"/>
       <c r="B61" s="2"/>
       <c r="C61" s="6"/>
@@ -1184,10 +1253,11 @@
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="6"/>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="H61" s="6"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="6"/>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="6"/>
       <c r="B62" s="2"/>
       <c r="C62" s="6"/>
@@ -1195,10 +1265,11 @@
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="6"/>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="H62" s="6"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="6"/>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="6"/>
       <c r="B63" s="2"/>
       <c r="C63" s="6"/>
@@ -1206,10 +1277,11 @@
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="6"/>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="H63" s="6"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="6"/>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="6"/>
       <c r="B64" s="2"/>
       <c r="C64" s="6"/>
@@ -1217,10 +1289,11 @@
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="6"/>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="H64" s="6"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="6"/>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="6"/>
       <c r="B65" s="2"/>
       <c r="C65" s="6"/>
@@ -1228,10 +1301,11 @@
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="6"/>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="H65" s="6"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="6"/>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" s="6"/>
       <c r="B66" s="2"/>
       <c r="C66" s="6"/>
@@ -1239,10 +1313,11 @@
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="6"/>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="H66" s="6"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="6"/>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="6"/>
       <c r="B67" s="2"/>
       <c r="C67" s="6"/>
@@ -1250,10 +1325,11 @@
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="6"/>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="H67" s="6"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="6"/>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" s="6"/>
       <c r="B68" s="2"/>
       <c r="C68" s="6"/>
@@ -1261,10 +1337,11 @@
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="6"/>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="H68" s="6"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="6"/>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" s="6"/>
       <c r="B69" s="2"/>
       <c r="C69" s="6"/>
@@ -1272,10 +1349,11 @@
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="6"/>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="H69" s="6"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="6"/>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="6"/>
       <c r="B70" s="2"/>
       <c r="C70" s="6"/>
@@ -1283,10 +1361,11 @@
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="6"/>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="H70" s="6"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="6"/>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" s="6"/>
       <c r="B71" s="2"/>
       <c r="C71" s="6"/>
@@ -1294,10 +1373,11 @@
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="6"/>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="H71" s="6"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="6"/>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" s="6"/>
       <c r="B72" s="2"/>
       <c r="C72" s="6"/>
@@ -1305,10 +1385,11 @@
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="6"/>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="H72" s="6"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="6"/>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" s="6"/>
       <c r="B73" s="2"/>
       <c r="C73" s="6"/>
@@ -1316,10 +1397,11 @@
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="6"/>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="H73" s="6"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="6"/>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" s="6"/>
       <c r="B74" s="2"/>
       <c r="C74" s="6"/>
@@ -1327,10 +1409,11 @@
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="6"/>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="H74" s="6"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="6"/>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" s="6"/>
       <c r="B75" s="2"/>
       <c r="C75" s="6"/>
@@ -1338,10 +1421,11 @@
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="6"/>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="H75" s="6"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="6"/>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" s="6"/>
       <c r="B76" s="2"/>
       <c r="C76" s="6"/>
@@ -1349,10 +1433,11 @@
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="6"/>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="H76" s="6"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="6"/>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" s="6"/>
       <c r="B77" s="2"/>
       <c r="C77" s="6"/>
@@ -1360,10 +1445,11 @@
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="6"/>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="H77" s="6"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="6"/>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" s="6"/>
       <c r="B78" s="2"/>
       <c r="C78" s="6"/>
@@ -1371,10 +1457,11 @@
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="6"/>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="H78" s="6"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="6"/>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" s="6"/>
       <c r="B79" s="2"/>
       <c r="C79" s="6"/>
@@ -1382,10 +1469,11 @@
       <c r="E79" s="6"/>
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="6"/>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="H79" s="6"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="6"/>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" s="6"/>
       <c r="B80" s="2"/>
       <c r="C80" s="6"/>
@@ -1393,10 +1481,11 @@
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="6"/>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="H80" s="6"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="6"/>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" s="6"/>
       <c r="B81" s="2"/>
       <c r="C81" s="6"/>
@@ -1404,10 +1493,11 @@
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="6"/>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="H81" s="6"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="6"/>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" s="6"/>
       <c r="B82" s="2"/>
       <c r="C82" s="6"/>
@@ -1415,10 +1505,11 @@
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="6"/>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="H82" s="6"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="6"/>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="6"/>
       <c r="B83" s="2"/>
       <c r="C83" s="6"/>
@@ -1426,10 +1517,11 @@
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="6"/>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="H83" s="6"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="6"/>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" s="6"/>
       <c r="B84" s="2"/>
       <c r="C84" s="6"/>
@@ -1437,10 +1529,11 @@
       <c r="E84" s="6"/>
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="6"/>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="H84" s="6"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="6"/>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" s="6"/>
       <c r="B85" s="2"/>
       <c r="C85" s="6"/>
@@ -1448,10 +1541,11 @@
       <c r="E85" s="6"/>
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="6"/>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="H85" s="6"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="6"/>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" s="6"/>
       <c r="B86" s="2"/>
       <c r="C86" s="6"/>
@@ -1459,10 +1553,11 @@
       <c r="E86" s="6"/>
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="6"/>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="H86" s="6"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="6"/>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" s="6"/>
       <c r="B87" s="2"/>
       <c r="C87" s="6"/>
@@ -1470,10 +1565,11 @@
       <c r="E87" s="6"/>
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="6"/>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="H87" s="6"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="6"/>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" s="6"/>
       <c r="B88" s="2"/>
       <c r="C88" s="6"/>
@@ -1481,10 +1577,11 @@
       <c r="E88" s="6"/>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="6"/>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="H88" s="6"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="6"/>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" s="6"/>
       <c r="B89" s="2"/>
       <c r="C89" s="6"/>
@@ -1492,10 +1589,11 @@
       <c r="E89" s="6"/>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="6"/>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="H89" s="6"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="6"/>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" s="6"/>
       <c r="B90" s="2"/>
       <c r="C90" s="6"/>
@@ -1503,10 +1601,11 @@
       <c r="E90" s="6"/>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="6"/>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="H90" s="6"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="6"/>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91" s="6"/>
       <c r="B91" s="2"/>
       <c r="C91" s="6"/>
@@ -1514,10 +1613,11 @@
       <c r="E91" s="6"/>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
-      <c r="H91" s="2"/>
-      <c r="I91" s="6"/>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="H91" s="6"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="6"/>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92" s="6"/>
       <c r="B92" s="2"/>
       <c r="C92" s="6"/>
@@ -1525,10 +1625,11 @@
       <c r="E92" s="6"/>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="6"/>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="H92" s="6"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="6"/>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93" s="6"/>
       <c r="B93" s="2"/>
       <c r="C93" s="6"/>
@@ -1536,10 +1637,11 @@
       <c r="E93" s="6"/>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="6"/>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="H93" s="6"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="6"/>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" s="6"/>
       <c r="B94" s="2"/>
       <c r="C94" s="6"/>
@@ -1547,10 +1649,11 @@
       <c r="E94" s="6"/>
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="6"/>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="H94" s="6"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="6"/>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" s="6"/>
       <c r="B95" s="2"/>
       <c r="C95" s="6"/>
@@ -1558,10 +1661,11 @@
       <c r="E95" s="6"/>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
-      <c r="H95" s="2"/>
-      <c r="I95" s="6"/>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="H95" s="6"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="6"/>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96" s="6"/>
       <c r="B96" s="2"/>
       <c r="C96" s="6"/>
@@ -1569,8 +1673,9 @@
       <c r="E96" s="6"/>
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>